<commit_message>
Minor edit: Exporting tables for appendix
</commit_message>
<xml_diff>
--- a/Output/Table1.xlsx
+++ b/Output/Table1.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -413,25 +413,25 @@
         </is>
       </c>
       <c r="B2" s="2">
-        <v>43915</v>
+        <v>43919</v>
       </c>
       <c r="C2">
-        <v>0.005738527141330698</v>
+        <v>0.006754162448951098</v>
       </c>
       <c r="D2">
-        <v>0.008215687128642849</v>
+        <v>0.009464650821448846</v>
       </c>
       <c r="E2">
-        <v>0.002144398024504367</v>
+        <v>-0.0004602093717535852</v>
       </c>
       <c r="F2">
-        <v>0.006071289104138482</v>
+        <v>0.009924860193202432</v>
       </c>
       <c r="G2">
-        <v>0.2610126202382052</v>
+        <v>0.0443145198859854</v>
       </c>
       <c r="H2">
-        <v>0.7389873797617947</v>
+        <v>0.9556854801140146</v>
       </c>
     </row>
     <row r="3">
@@ -447,19 +447,19 @@
         <v>0.01227108704745637</v>
       </c>
       <c r="D3">
-        <v>0.00168312722251718</v>
+        <v>0.003947726222943577</v>
       </c>
       <c r="E3">
-        <v>-0.0002386230963777816</v>
+        <v>-0.0001608464805649595</v>
       </c>
       <c r="F3">
-        <v>0.001921750318894962</v>
+        <v>0.004108572703508538</v>
       </c>
       <c r="G3">
-        <v>0.1104545606286568</v>
+        <v>0.03767408952603575</v>
       </c>
       <c r="H3">
-        <v>0.8895454393713432</v>
+        <v>0.9623259104739642</v>
       </c>
     </row>
     <row r="4">
@@ -469,10 +469,10 @@
         </is>
       </c>
       <c r="B4" s="2">
-        <v>43916</v>
+        <v>43920</v>
       </c>
       <c r="C4">
-        <v>0.01395421426997355</v>
+        <v>0.01621881327039994</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -497,19 +497,19 @@
         <v>0.01732289677803195</v>
       </c>
       <c r="D5">
-        <v>-0.003368682508058406</v>
+        <v>-0.001104083507632008</v>
       </c>
       <c r="E5">
-        <v>-0.009905958297177265</v>
+        <v>-0.01130159718274817</v>
       </c>
       <c r="F5">
-        <v>0.006537275789118861</v>
+        <v>0.01019751367511616</v>
       </c>
       <c r="G5">
-        <v>0.6024336967526931</v>
+        <v>0.5256774225439219</v>
       </c>
       <c r="H5">
-        <v>0.3975663032473071</v>
+        <v>0.474322577456078</v>
       </c>
     </row>
     <row r="6">
@@ -525,19 +525,19 @@
         <v>0.02276530386775508</v>
       </c>
       <c r="D6">
-        <v>-0.008811089597781534</v>
+        <v>-0.006546490597355136</v>
       </c>
       <c r="E6">
-        <v>-0.001222002665949007</v>
+        <v>-0.0009030758576810743</v>
       </c>
       <c r="F6">
-        <v>-0.007589086931832525</v>
+        <v>-0.005643414739674061</v>
       </c>
       <c r="G6">
-        <v>0.138689165782253</v>
+        <v>0.1379480874907127</v>
       </c>
       <c r="H6">
-        <v>0.8613108342177471</v>
+        <v>0.8620519125092873</v>
       </c>
     </row>
     <row r="7">
@@ -547,81 +547,109 @@
         </is>
       </c>
       <c r="B7" s="2">
-        <v>43905</v>
+        <v>43914</v>
       </c>
       <c r="C7">
-        <v>0.02620742418467345</v>
+        <v>0.03983587515221891</v>
       </c>
       <c r="D7">
-        <v>-0.01225320991469991</v>
+        <v>-0.02361706188181897</v>
       </c>
       <c r="E7">
-        <v>-0.01539889014453901</v>
+        <v>-0.02098271874324288</v>
       </c>
       <c r="F7">
-        <v>0.003145680229839099</v>
+        <v>-0.002634343138576091</v>
       </c>
       <c r="G7">
-        <v>0.830371900435866</v>
+        <v>0.8884559327591854</v>
       </c>
       <c r="H7">
-        <v>0.169628099564134</v>
+        <v>0.1115440672408145</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>USA_WA</t>
         </is>
       </c>
       <c r="B8" s="2">
-        <v>43915</v>
+        <v>43919</v>
       </c>
       <c r="C8">
-        <v>0.07277354595287251</v>
+        <v>0.04349561395511622</v>
       </c>
       <c r="D8">
-        <v>-0.05881933168289896</v>
+        <v>-0.02727680068471627</v>
       </c>
       <c r="E8">
-        <v>-0.03356800370397964</v>
+        <v>-0.01993017427657376</v>
       </c>
       <c r="F8">
-        <v>-0.02525132797891931</v>
+        <v>-0.007346626408142511</v>
       </c>
       <c r="G8">
-        <v>0.5706967886841726</v>
+        <v>0.7306639259838501</v>
       </c>
       <c r="H8">
-        <v>0.4293032113158274</v>
+        <v>0.26933607401615</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>Spain</t>
+        </is>
+      </c>
+      <c r="B9" s="2">
+        <v>43919</v>
+      </c>
+      <c r="C9">
+        <v>0.08615529080345091</v>
+      </c>
+      <c r="D9">
+        <v>-0.06993647753305096</v>
+      </c>
+      <c r="E9">
+        <v>-0.03964027430057621</v>
+      </c>
+      <c r="F9">
+        <v>-0.03029620323247475</v>
+      </c>
+      <c r="G9">
+        <v>0.5668039869729326</v>
+      </c>
+      <c r="H9">
+        <v>0.4331960130270674</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
           <t>Italy</t>
         </is>
       </c>
-      <c r="B9" s="2">
-        <v>43916</v>
-      </c>
-      <c r="C9">
-        <v>0.09630539297713012</v>
-      </c>
-      <c r="D9">
-        <v>-0.08235117870715657</v>
-      </c>
-      <c r="E9">
-        <v>-0.04561535718713806</v>
-      </c>
-      <c r="F9">
-        <v>-0.03673582152001852</v>
-      </c>
-      <c r="G9">
-        <v>0.5539126203566281</v>
-      </c>
-      <c r="H9">
-        <v>0.4460873796433718</v>
+      <c r="B10" s="2">
+        <v>43919</v>
+      </c>
+      <c r="C10">
+        <v>0.1063320056230004</v>
+      </c>
+      <c r="D10">
+        <v>-0.09011319235260046</v>
+      </c>
+      <c r="E10">
+        <v>-0.0518290945368735</v>
+      </c>
+      <c r="F10">
+        <v>-0.03828409781572694</v>
+      </c>
+      <c r="G10">
+        <v>0.5751554593035994</v>
+      </c>
+      <c r="H10">
+        <v>0.4248445406964007</v>
       </c>
     </row>
   </sheetData>

</xml_diff>